<commit_message>
Update bar plot preparation directions in a markdown file
</commit_message>
<xml_diff>
--- a/data/Economist_Charts.xlsx
+++ b/data/Economist_Charts.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B7D909B-42BA-3445-8C9E-8D20A73C0FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FB5E40-9276-7948-8997-D08DC19D1207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="940" windowWidth="24420" windowHeight="16380" xr2:uid="{BAB1E410-742B-4976-960A-2ACD449F15F7}"/>
+    <workbookView xWindow="12600" yWindow="1280" windowWidth="28720" windowHeight="16380" xr2:uid="{BAB1E410-742B-4976-960A-2ACD449F15F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Template Chart 1" sheetId="9" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -239,10 +238,10 @@
     <t>labels</t>
   </si>
   <si>
-    <t>Manufacturing company sourcing parts from Chine &amp; US</t>
+    <t>Battery cells</t>
   </si>
   <si>
-    <t>Battery cells</t>
+    <t>Manufacturing company sourcing parts from China &amp; US</t>
   </si>
 </sst>
 </file>
@@ -590,8 +589,8 @@
   <colors>
     <mruColors>
       <color rgb="FFEE422A"/>
+      <color rgb="FFDE140C"/>
       <color rgb="FFFF7575"/>
-      <color rgb="FFDE140C"/>
       <color rgb="FFB3B19C"/>
       <color rgb="FFDBDACF"/>
       <color rgb="FFCFCDBF"/>
@@ -1106,6 +1105,498 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Template Chart 1'!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>China</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="EE422A"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Template Chart 1'!$A$6:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Battery cells</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Microprocessors</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>LCD Displays</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sensors</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>HPC chips</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Template Chart 1'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-60EB-1C4E-A698-77E2DA004699}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Template Chart 1'!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>United States</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="0">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="r">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Template Chart 1'!$A$6:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Battery cells</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Microprocessors</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>LCD Displays</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sensors</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>HPC chips</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Template Chart 1'!$C$6:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>291</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>988</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>689</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-60EB-1C4E-A698-77E2DA004699}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="226742880"/>
+        <c:axId val="226744608"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="226742880"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226744608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="226744608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="226742880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.65961067366579174"/>
+          <c:y val="9.9592578072661087E-2"/>
+          <c:w val="0.29744510061242346"/>
+          <c:h val="6.2560881948642719E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -1536,7 +2027,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D23D5B0B-D08B-D44C-AC9E-159C9684B0EE}" type="CELLRANGE">
+                    <a:fld id="{08841AD3-0117-934B-839F-3B168A2D8AC8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1570,7 +2061,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03DAFFA7-72DC-F347-9CA8-B0D764C65D40}" type="CELLRANGE">
+                    <a:fld id="{60F34834-907D-DB43-83DC-938F7C01F551}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1604,7 +2095,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4CC0B687-DFDD-FE4A-884B-3BBB7BABCA06}" type="CELLRANGE">
+                    <a:fld id="{67792B38-5691-E04E-919B-F8F536423005}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1638,7 +2129,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9478CBD9-A154-1645-89DE-4DEE77881AF4}" type="CELLRANGE">
+                    <a:fld id="{02918403-D439-3F4A-86D1-158EEBDE2C82}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1672,7 +2163,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A49B985-BE0F-CD43-845E-BC42590CDCB4}" type="CELLRANGE">
+                    <a:fld id="{81561B34-B54F-4D4C-8BAC-E1D49EC76D2D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1706,7 +2197,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B457A1D5-C931-F64C-8141-D6AA2073CA96}" type="CELLRANGE">
+                    <a:fld id="{F9B8C18F-8655-E345-941A-8D3500431BAB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1740,7 +2231,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5733F505-11B5-0843-8D57-DB9BA476EF26}" type="CELLRANGE">
+                    <a:fld id="{34B35725-6710-0B4F-803B-D7BBB8B898FA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1774,7 +2265,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFC287D4-2823-B148-8266-3886F5B4CEDB}" type="CELLRANGE">
+                    <a:fld id="{CCB3FA67-4456-6940-8E76-C6437BCB88AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2196,6 +2687,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -2702,6 +3233,511 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3250,6 +4286,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>259521</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>115956</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>176695</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AD442A2-D3B9-2F4A-3680-87FCC9B17477}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4383,7 +5455,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -4396,7 +5468,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.75" customHeight="1"/>
@@ -4415,7 +5487,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>370</v>

</xml_diff>